<commit_message>
EU Industry now builds
</commit_message>
<xml_diff>
--- a/data/steel/steel_industry_EU28.xlsx
+++ b/data/steel/steel_industry_EU28.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="165" yWindow="465" windowWidth="25260" windowHeight="15765"/>
+    <workbookView xWindow="165" yWindow="465" windowWidth="25260" windowHeight="15765" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Factory List" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="2050" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,9 +61,6 @@
     <t>EUROFER 2010</t>
   </si>
   <si>
-    <t>EUROFER 2030_Economic</t>
-  </si>
-  <si>
     <t>BF-BOF</t>
   </si>
   <si>
@@ -113,27 +109,6 @@
     <t>BF-BOF bio w CCS BF CO</t>
   </si>
   <si>
-    <t>steel_simplified_EAF.xlsx</t>
-  </si>
-  <si>
-    <t>steel_simplified_factory.xlsx</t>
-  </si>
-  <si>
-    <t>bb_steel_factories.xlsx</t>
-  </si>
-  <si>
-    <t>steel_simplified_factory-ccs.xlsx</t>
-  </si>
-  <si>
-    <t>.xlsxsteel_simplified_factory-ccs-bfcoke</t>
-  </si>
-  <si>
-    <t>steel_simplified_factory-ccs-bfonly.xlsx</t>
-  </si>
-  <si>
-    <t>steel_simplified_factory-ccs-bfcoke.xlsx</t>
-  </si>
-  <si>
     <t>chains</t>
   </si>
   <si>
@@ -150,6 +125,30 @@
   </si>
   <si>
     <t>bf-eaf connections</t>
+  </si>
+  <si>
+    <t>C:\Users\setanzer\GitHub\BlackBlox\data\steel\steel_simplified_factory.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\setanzer\GitHub\BlackBlox\data\steel\steel_simplified_EAF.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\setanzer\GitHub\BlackBlox\data\steel\bb_steel_factories.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\setanzer\GitHub\BlackBlox\data\steel\steel_simplified_factory-ccs.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\setanzer\GitHub\BlackBlox\data\steel\steel_simplified_factory-ccs-bfonly.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\setanzer\GitHub\BlackBlox\data\steel\steel_simplified_factory-ccs-bfcoke.xlsx</t>
+  </si>
+  <si>
+    <t>crude steel</t>
+  </si>
+  <si>
+    <t>EU-EAF-base-2030</t>
   </si>
 </sst>
 </file>
@@ -511,14 +510,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.875" customWidth="1"/>
     <col min="4" max="4" width="25.125" customWidth="1"/>
   </cols>
@@ -539,142 +538,142 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -687,7 +686,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -711,12 +710,12 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -763,12 +762,12 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -791,7 +790,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -815,41 +814,41 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>100.864</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>65.247</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -862,7 +861,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -887,58 +886,58 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <f>(204-$C$3)*0.8</f>
         <v>94.656000000000006</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <f>204*0.42</f>
         <v>85.679999999999993</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <f>(204-$C$3)*0.2</f>
         <v>23.664000000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -950,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -975,40 +974,40 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <f>247*0.44</f>
         <v>108.68</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <f>247-C2</f>
         <v>138.32</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>